<commit_message>
GameServerPlacesUpdater.py added default name for the sheets
</commit_message>
<xml_diff>
--- a/BrainServer/dist/results_example.xlsx
+++ b/BrainServer/dist/results_example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\timeo\PycharmProjects\SilaMisli2025\V1\BrainServer\dist\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D1BA759-3FB1-440C-B0A4-8FE553154E5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AAC4399-B77E-4B38-B1C7-A5641AE16AAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="34">
   <si>
     <t>ИТОГ</t>
   </si>
@@ -143,6 +143,10 @@
     <t>Collects the teams list from the column 'B' and depends of them order in the list a team will be selected
  to be writen down to the related "places" in the PowerPoint file
  (the rouls and the place names defined in the places.json config file accordingly)</t>
+  </si>
+  <si>
+    <t>If in an Excel file, there are many sheets, then set the sheet name as here: 'Таблица на экран'==&gt;'AllResultsOnTable'.
+It will guarantee that the expected data will be found accordingly.</t>
   </si>
 </sst>
 </file>
@@ -280,7 +284,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -308,6 +312,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -348,7 +358,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -449,6 +459,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -8278,10 +8291,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{089F9DF6-D74B-475A-B4F8-F836C2F9A564}">
-  <dimension ref="F1:F2"/>
+  <dimension ref="F1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8299,6 +8312,11 @@
         <v>32</v>
       </c>
     </row>
+    <row r="3" spans="6:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="F3" s="40" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>